<commit_message>
Update summary.py with diaries statistics
</commit_message>
<xml_diff>
--- a/men_diaries/Diary 10 (Igor).xlsx
+++ b/men_diaries/Diary 10 (Igor).xlsx
@@ -13,23 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="99">
-  <si>
-    <t xml:space="preserve">(i) The motivations of females to use technology are more likely to be for what it helps them accomplish, whereas for males more likely to be for their interest and enjoyment of technology itself 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(ii) Females statistically have lower computer self-efficacy (confidence) than males within their peer sets, which can affect their behavior with technology
-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="99">
   <si>
     <t>[Newcomer's Orientation] Finding a task to start with</t>
   </si>
   <si>
-    <t>(iii) Females tend to be more risk-averse than males,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(iv) More females than males process information comprehensively — gathering fairly complete information before proceeding — but more males than females use selective styles — following the first promising information, then backtracking if needed </t>
+    <t xml:space="preserve">(i) The motivations of females to use technology are more likely to be for what it helps them accomplish, whereas for males more likely to be for their interest and enjoyment of technology itself 
+</t>
   </si>
   <si>
     <t>[Newcomer's Orientation] Finding a mentor</t>
@@ -45,35 +35,27 @@
 Newcomer's Behavior] Lack of Patience</t>
   </si>
   <si>
-    <t>(v) Females are more likely to prefer learning software features in process-oriented learning styles and less likely than males to prefer learning new software features by playfully experimenting</t>
+    <t xml:space="preserve">(ii) Females statistically have lower computer self-efficacy (confidence) than males within their peer sets, which can affect their behavior with technology
+</t>
   </si>
   <si>
-    <t>[Newcomer's characteristics - Newcomer's Communication] Shyness</t>
+    <t>(iii) Females tend to be more risk-averse than males,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(iv) More females than males process information comprehensively — gathering fairly complete information before proceeding — but more males than females use selective styles — following the first promising information, then backtracking if needed </t>
+  </si>
+  <si>
+    <t>(v) Females are more likely to prefer learning software features in process-oriented learning styles and less likely than males to prefer learning new software features by playfully experimenting</t>
   </si>
   <si>
     <t xml:space="preserve">Today I officially started my journey in an attempt to contribute to a open source project. For me, the idea sounds very interesting: I've been using GNU / Linux for over fifteen years and I've been in the communities of some distros, but I've never been directly involved with bug reporting, nor have I contributed with code. I always thought that I did not have the technical ability to do that.
 </t>
   </si>
   <si>
-    <t>[Newcomers' characteristics - Newcomer's Previous Knowledge] Lack of domain expertise</t>
-  </si>
-  <si>
     <t>A-</t>
   </si>
   <si>
     <t>I have now been assigned the task of (trying) to implement a new functionality or to fix a bug on Empathy. I confess that the software choice is not particularly of my interest. Also, among all open Instant Messaging programs, Empathy is probably what I least know about. I've already used Pidgin, Ekiga, Kopete, and the (almosted) dead MSN Messenger.</t>
-  </si>
-  <si>
-    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge] Lack of knowledge in project processes and practice</t>
-  </si>
-  <si>
-    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge - Lack of technical background] Knowledge on technologies and tools used</t>
-  </si>
-  <si>
-    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge - Lack of technical background] Knowledge of versioning control systems</t>
-  </si>
-  <si>
-    <t>[Reception Issues] Receiving answers with too advanced/complex contents</t>
   </si>
   <si>
     <t xml:space="preserve">Let's take a brief summary of what I discovered or remembered about Empathy by searching the internet:
@@ -91,18 +73,6 @@
     <t xml:space="preserve">After seeking to know more about Empathy, I tried to find out how I would contribute to the project. So far I had spent a few hours, I spent more hours trying to figure out how newcomers could contribute. </t>
   </si>
   <si>
-    <t>[Reception Issues] Impolite answers</t>
-  </si>
-  <si>
-    <t>[Reception Issues] Not receiving an answer</t>
-  </si>
-  <si>
-    <t>[Reception Issues] Delayed Answer</t>
-  </si>
-  <si>
-    <t>[Cultural Differences] Some newcomers need to contact a real person</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unfortunately, some contribution pages have been out of date for more than two years. However, at least some people seem to be very receptive and willing to help you, like this Empathy mentor: http://chandniverma.blogspot.com.br/
 </t>
   </si>
@@ -111,29 +81,11 @@
 </t>
   </si>
   <si>
-    <t>[Documentation Problems] Outdated</t>
-  </si>
-  <si>
     <t>I must have spent about one hour doing this. I followed the recommended steps from https://wiki.gnome.org/GnomeLove/Mentors and I tried to talk with Guillaume Desmottes using IRC, who ignored me for the time I was online on the GIMPNet #empathy channel. Maybe he was away, or maybe he didn’t want to waste time with an stranger. Unfortunately, he was the only mentor online.</t>
   </si>
   <si>
     <t xml:space="preserve">I also spent an hour looking for feasible bugs, that is, bugs that can be solved by someone who clearly lacks the expertise to handle with a software with more than 100 thousand lines of code, without any documentation for developers.
 </t>
-  </si>
-  <si>
-    <t>[Documentation Problems] Overload</t>
-  </si>
-  <si>
-    <t>[Documentation Problems] Unclear</t>
-  </si>
-  <si>
-    <t>[Documentation Problems] Spread</t>
-  </si>
-  <si>
-    <t>[Documentation Problems - Lack of Documentation] General</t>
-  </si>
-  <si>
-    <t>[Technical Hurdles - Local environment setup hurdles] Building workspace locally</t>
   </si>
   <si>
     <t xml:space="preserve"> In this case, Gnome recommends that I look for bugs marked as “gnome-love”. That is what I did.</t>
@@ -145,17 +97,8 @@
     <t>All the other bugs are from three, four or five years ago, of discontinued versions. Even if they are open, does anyone still expect fixes for them?</t>
   </si>
   <si>
-    <t>[Technical Hurdles - Change request hurdles] Lack of information on how to send a contribution</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anyway, I cloned Empathy's repository and started to study the code. Honestly, knowing C does not help much. You need to be familiar with the Telepathy API, as well as GObject and GTK.
 </t>
-  </si>
-  <si>
-    <t>[Technical Hurdles - Change request hurdles] Getting contribution accepted</t>
-  </si>
-  <si>
-    <t>[Technical Hurdles - Change request hurdles] Issue to create a patch</t>
   </si>
   <si>
     <t>Today I joined a roommate to see if together we could get people's attention on the Empathy channel on GIMPNet. We posted IRC messages, but just like yesterday, no one answered.</t>
@@ -206,9 +149,6 @@
   <si>
     <t xml:space="preserve">As I understand it, GObject is not only a way of creating object orientation in C, but also something necessary from the integration point of view. The types in GObjects are basically GLib types and macros.
 </t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>It may seem like a small discovery, but it made me realize how we undergraduates do not pay attention to problems related to cross-compiling and software integration.</t>
@@ -369,6 +309,66 @@
     <t xml:space="preserve">In the end, it may have been just bad luck. Everyone is temporarily busy and someday everything will return to normal. In any case, I will end the diary with the same convictions with which I began the work. I still believe that the idea of ​​contributing to a free software project is great. I still enjoy the spirit that permeates community development. And I keep using Pidgin as a chat software.
 </t>
   </si>
+  <si>
+    <t>[Newcomer's characteristics - Newcomer's Communication] Shyness</t>
+  </si>
+  <si>
+    <t>[Newcomers' characteristics - Newcomer's Previous Knowledge] Lack of domain expertise</t>
+  </si>
+  <si>
+    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge] Lack of knowledge in project processes and practice</t>
+  </si>
+  <si>
+    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge - Lack of technical background] Knowledge on technologies and tools used</t>
+  </si>
+  <si>
+    <t>[Newcomer's characteristics - Newcomer's Previous Knowledge - Lack of technical background] Knowledge of versioning control systems</t>
+  </si>
+  <si>
+    <t>[Reception Issues] Receiving answers with too advanced/complex contents</t>
+  </si>
+  <si>
+    <t>[Reception Issues] Impolite answers</t>
+  </si>
+  <si>
+    <t>[Reception Issues] Not receiving an answer</t>
+  </si>
+  <si>
+    <t>[Reception Issues] Delayed Answer</t>
+  </si>
+  <si>
+    <t>[Cultural Differences] Some newcomers need to contact a real person</t>
+  </si>
+  <si>
+    <t>[Documentation Problems] Outdated</t>
+  </si>
+  <si>
+    <t>[Documentation Problems] Overload</t>
+  </si>
+  <si>
+    <t>[Documentation Problems] Unclear</t>
+  </si>
+  <si>
+    <t>[Documentation Problems] Spread</t>
+  </si>
+  <si>
+    <t>[Documentation Problems - Lack of Documentation] General</t>
+  </si>
+  <si>
+    <t>[Technical Hurdles - Local environment setup hurdles] Building workspace locally</t>
+  </si>
+  <si>
+    <t>[Technical Hurdles - Change request hurdles] Lack of information on how to send a contribution</t>
+  </si>
+  <si>
+    <t>[Technical Hurdles - Change request hurdles] Getting contribution accepted</t>
+  </si>
+  <si>
+    <t>[Technical Hurdles - Change request hurdles] Issue to create a patch</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
@@ -398,6 +398,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF6FA8DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFD966"/>
         <bgColor rgb="FFFFD966"/>
       </patternFill>
@@ -412,12 +418,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
         <bgColor rgb="FFC9DAF8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6FA8DC"/>
-        <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
     <fill>
@@ -464,8 +464,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -473,25 +473,25 @@
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -513,10 +513,10 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,83 +562,83 @@
   <sheetData>
     <row r="1" ht="186.0" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>10</v>
+      <c r="G1" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="Z1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -647,14 +647,16 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -684,7 +686,7 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -697,11 +699,11 @@
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="V5" s="18"/>
+      <c r="V5" s="19"/>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -717,7 +719,7 @@
     </row>
     <row r="7">
       <c r="A7" s="16" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -730,14 +732,14 @@
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="Q7" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="V7" s="18"/>
+      <c r="Q7" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="V7" s="19"/>
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -753,11 +755,11 @@
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="19" t="s">
-        <v>56</v>
+      <c r="C9" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -768,19 +770,19 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="N9" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P9" s="18" t="s">
-        <v>56</v>
+      <c r="N9" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>56</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -792,13 +794,13 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
-      <c r="U10" s="18" t="s">
-        <v>56</v>
+      <c r="U10" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -814,10 +816,10 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -832,7 +834,7 @@
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -848,7 +850,7 @@
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -858,15 +860,15 @@
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="19" t="s">
-        <v>56</v>
+      <c r="J14" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -879,16 +881,16 @@
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
-      <c r="N15" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P15" s="18" t="s">
-        <v>56</v>
+      <c r="N15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -901,16 +903,16 @@
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
-      <c r="N16" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P16" s="18" t="s">
-        <v>56</v>
+      <c r="N16" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -923,13 +925,13 @@
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
-      <c r="N17" s="18" t="s">
-        <v>56</v>
+      <c r="N17" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -945,7 +947,7 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -961,7 +963,7 @@
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -971,15 +973,15 @@
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="19" t="s">
-        <v>56</v>
+      <c r="J20" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -995,7 +997,7 @@
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1011,7 +1013,7 @@
     </row>
     <row r="23">
       <c r="A23" s="16" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1027,7 +1029,7 @@
     </row>
     <row r="24">
       <c r="A24" s="16" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1043,7 +1045,7 @@
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1059,7 +1061,7 @@
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1075,7 +1077,7 @@
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1091,7 +1093,7 @@
     </row>
     <row r="28">
       <c r="A28" s="16" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1107,7 +1109,7 @@
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1123,7 +1125,7 @@
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1139,7 +1141,7 @@
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1152,10 +1154,13 @@
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
+      <c r="U31" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>62</v>
+      <c r="A32" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1170,8 +1175,8 @@
       <c r="L32" s="17"/>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>63</v>
+      <c r="A33" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -1186,8 +1191,8 @@
       <c r="L33" s="17"/>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="s">
-        <v>64</v>
+      <c r="A34" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -1202,8 +1207,8 @@
       <c r="L34" s="17"/>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="s">
-        <v>65</v>
+      <c r="A35" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -1218,8 +1223,8 @@
       <c r="L35" s="17"/>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="s">
-        <v>66</v>
+      <c r="A36" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -1234,8 +1239,8 @@
       <c r="L36" s="17"/>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="s">
-        <v>67</v>
+      <c r="A37" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1250,8 +1255,8 @@
       <c r="L37" s="17"/>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="s">
-        <v>68</v>
+      <c r="A38" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -1264,13 +1269,13 @@
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
-      <c r="V38" s="18" t="s">
-        <v>56</v>
+      <c r="V38" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
-        <v>69</v>
+      <c r="A39" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -1285,8 +1290,8 @@
       <c r="L39" s="17"/>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
-        <v>70</v>
+      <c r="A40" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -1299,13 +1304,13 @@
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
-      <c r="V40" s="18" t="s">
-        <v>56</v>
+      <c r="V40" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="s">
-        <v>71</v>
+      <c r="A41" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1320,8 +1325,8 @@
       <c r="L41" s="17"/>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="s">
-        <v>72</v>
+      <c r="A42" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -1329,8 +1334,8 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
-      <c r="H42" s="19" t="s">
-        <v>56</v>
+      <c r="H42" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
@@ -1338,8 +1343,8 @@
       <c r="L42" s="17"/>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="s">
-        <v>73</v>
+      <c r="A43" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -1354,8 +1359,8 @@
       <c r="L43" s="17"/>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="s">
-        <v>74</v>
+      <c r="A44" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
@@ -1370,8 +1375,8 @@
       <c r="L44" s="17"/>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="s">
-        <v>75</v>
+      <c r="A45" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -1379,8 +1384,8 @@
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
-      <c r="H45" s="19" t="s">
-        <v>56</v>
+      <c r="H45" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="I45" s="17"/>
       <c r="J45" s="17"/>
@@ -1388,8 +1393,8 @@
       <c r="L45" s="17"/>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="s">
-        <v>76</v>
+      <c r="A46" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -1404,8 +1409,8 @@
       <c r="L46" s="17"/>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>77</v>
+      <c r="A47" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -1420,8 +1425,8 @@
       <c r="L47" s="17"/>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="s">
-        <v>78</v>
+      <c r="A48" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -1436,8 +1441,8 @@
       <c r="L48" s="17"/>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="s">
-        <v>79</v>
+      <c r="A49" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -1450,13 +1455,13 @@
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
-      <c r="W49" s="18" t="s">
-        <v>56</v>
+      <c r="W49" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="s">
-        <v>80</v>
+      <c r="A50" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -1469,16 +1474,16 @@
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
-      <c r="N50" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P50" s="18" t="s">
-        <v>56</v>
+      <c r="N50" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P50" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="s">
-        <v>81</v>
+      <c r="A51" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -1491,16 +1496,16 @@
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
-      <c r="N51" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P51" s="18" t="s">
-        <v>56</v>
+      <c r="N51" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P51" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="10" t="s">
-        <v>82</v>
+      <c r="A52" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -1515,8 +1520,8 @@
       <c r="L52" s="17"/>
     </row>
     <row r="53">
-      <c r="A53" s="10" t="s">
-        <v>83</v>
+      <c r="A53" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -1531,8 +1536,8 @@
       <c r="L53" s="17"/>
     </row>
     <row r="54">
-      <c r="A54" s="10" t="s">
-        <v>84</v>
+      <c r="A54" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -1547,8 +1552,8 @@
       <c r="L54" s="17"/>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="s">
-        <v>85</v>
+      <c r="A55" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -1563,8 +1568,8 @@
       <c r="L55" s="17"/>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
-        <v>86</v>
+      <c r="A56" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -1579,8 +1584,8 @@
       <c r="L56" s="17"/>
     </row>
     <row r="57">
-      <c r="A57" s="10" t="s">
-        <v>87</v>
+      <c r="A57" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -1593,16 +1598,16 @@
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
       <c r="L57" s="17"/>
-      <c r="N57" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="X57" s="18" t="s">
-        <v>56</v>
+      <c r="N57" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="X57" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="10" t="s">
-        <v>88</v>
+      <c r="A58" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -1617,8 +1622,8 @@
       <c r="L58" s="17"/>
     </row>
     <row r="59">
-      <c r="A59" s="10" t="s">
-        <v>89</v>
+      <c r="A59" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -1631,16 +1636,16 @@
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
-      <c r="N59" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="X59" s="18" t="s">
-        <v>56</v>
+      <c r="N59" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="X59" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="10" t="s">
-        <v>90</v>
+      <c r="A60" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -1653,16 +1658,16 @@
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
       <c r="L60" s="17"/>
-      <c r="N60" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="X60" s="18" t="s">
-        <v>56</v>
+      <c r="N60" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="X60" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="s">
-        <v>91</v>
+      <c r="A61" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -1677,8 +1682,8 @@
       <c r="L61" s="17"/>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="s">
-        <v>92</v>
+      <c r="A62" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -1693,8 +1698,8 @@
       <c r="L62" s="17"/>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
-        <v>93</v>
+      <c r="A63" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -1709,8 +1714,8 @@
       <c r="L63" s="17"/>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
-        <v>94</v>
+      <c r="A64" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -1723,16 +1728,16 @@
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
       <c r="L64" s="17"/>
-      <c r="N64" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="X64" s="18" t="s">
-        <v>56</v>
+      <c r="N64" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="X64" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="s">
-        <v>95</v>
+      <c r="A65" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -1747,24 +1752,28 @@
       <c r="L65" s="17"/>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="17"/>
-      <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
+      <c r="A66" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
-        <v>97</v>
+      <c r="A67" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -1777,10 +1786,13 @@
       <c r="J67" s="17"/>
       <c r="K67" s="17"/>
       <c r="L67" s="17"/>
+      <c r="N67" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="s">
-        <v>98</v>
+      <c r="A68" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -1793,11 +1805,11 @@
       <c r="J68" s="17"/>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
-      <c r="N68" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="X68" s="18" t="s">
-        <v>56</v>
+      <c r="N68" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="X68" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="69">
@@ -14868,37 +14880,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>14</v>
+      <c r="A3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -14907,7 +14919,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -14915,20 +14927,20 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>19</v>
+      <c r="A5" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
-        <v>20</v>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
+      <c r="A6" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -14937,8 +14949,8 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>26</v>
+      <c r="A7" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -14947,8 +14959,8 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>27</v>
+      <c r="A8" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -14957,20 +14969,20 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>29</v>
+      <c r="A9" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="10" t="s">
-        <v>13</v>
+      <c r="F9" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>30</v>
+      <c r="A10" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -14979,8 +14991,8 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>36</v>
+      <c r="A11" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -14989,8 +15001,8 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>37</v>
+      <c r="A12" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -14999,8 +15011,8 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="s">
-        <v>38</v>
+      <c r="A13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -15009,8 +15021,8 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>40</v>
+      <c r="A14" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -15019,8 +15031,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
-        <v>43</v>
+      <c r="A15" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -15029,8 +15041,8 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>44</v>
+      <c r="A16" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -15039,8 +15051,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>45</v>
+      <c r="A17" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -15049,8 +15061,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>46</v>
+      <c r="A18" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -15059,32 +15071,32 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
-        <v>47</v>
+      <c r="A19" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="10" t="s">
-        <v>20</v>
+      <c r="E19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>48</v>
+      <c r="A20" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="10" t="s">
-        <v>49</v>
+      <c r="E20" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>50</v>
+      <c r="A21" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -15093,8 +15105,8 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>51</v>
+      <c r="A22" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -15103,8 +15115,8 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>52</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -15113,8 +15125,8 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>53</v>
+      <c r="A24" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -15123,8 +15135,8 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>54</v>
+      <c r="A25" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -15133,8 +15145,8 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
-        <v>55</v>
+      <c r="A26" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -15143,8 +15155,8 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>57</v>
+      <c r="A27" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -15153,20 +15165,20 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="s">
-        <v>58</v>
+      <c r="A28" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="10" t="s">
-        <v>49</v>
+      <c r="E28" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
-        <v>59</v>
+      <c r="A29" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -15175,68 +15187,68 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>60</v>
+      <c r="A30" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="10" t="s">
-        <v>49</v>
+      <c r="E30" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>61</v>
+      <c r="A31" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="10"/>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>62</v>
+      <c r="A32" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="10" t="s">
-        <v>49</v>
+      <c r="F32" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>63</v>
+      <c r="A33" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="10" t="s">
-        <v>49</v>
+      <c r="F33" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="s">
-        <v>64</v>
+      <c r="A34" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="10" t="s">
-        <v>49</v>
+      <c r="F34" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="s">
-        <v>65</v>
+      <c r="A35" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -15245,8 +15257,8 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="s">
-        <v>66</v>
+      <c r="A36" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -15255,8 +15267,8 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="s">
-        <v>67</v>
+      <c r="A37" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -15265,8 +15277,8 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="s">
-        <v>68</v>
+      <c r="A38" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -15275,8 +15287,8 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
-        <v>69</v>
+      <c r="A39" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -15285,8 +15297,8 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
-        <v>70</v>
+      <c r="A40" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -15295,8 +15307,8 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="s">
-        <v>71</v>
+      <c r="A41" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -15305,8 +15317,8 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="s">
-        <v>72</v>
+      <c r="A42" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -15315,8 +15327,8 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="s">
-        <v>73</v>
+      <c r="A43" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -15325,8 +15337,8 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="s">
-        <v>74</v>
+      <c r="A44" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -15335,8 +15347,8 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="s">
-        <v>75</v>
+      <c r="A45" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -15345,8 +15357,8 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="s">
-        <v>76</v>
+      <c r="A46" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -15355,8 +15367,8 @@
       <c r="F46" s="1"/>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>77</v>
+      <c r="A47" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -15365,8 +15377,8 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="s">
-        <v>78</v>
+      <c r="A48" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -15375,8 +15387,8 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="s">
-        <v>79</v>
+      <c r="A49" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -15385,8 +15397,8 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="s">
-        <v>80</v>
+      <c r="A50" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -15395,8 +15407,8 @@
       <c r="F50" s="1"/>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="s">
-        <v>81</v>
+      <c r="A51" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -15405,8 +15417,8 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52">
-      <c r="A52" s="10" t="s">
-        <v>82</v>
+      <c r="A52" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -15415,8 +15427,8 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53">
-      <c r="A53" s="10" t="s">
-        <v>83</v>
+      <c r="A53" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -15425,8 +15437,8 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54">
-      <c r="A54" s="10" t="s">
-        <v>84</v>
+      <c r="A54" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -15435,8 +15447,8 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="s">
-        <v>85</v>
+      <c r="A55" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -15445,8 +15457,8 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
-        <v>86</v>
+      <c r="A56" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -15455,8 +15467,8 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57">
-      <c r="A57" s="10" t="s">
-        <v>87</v>
+      <c r="A57" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -15465,8 +15477,8 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58">
-      <c r="A58" s="10" t="s">
-        <v>88</v>
+      <c r="A58" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -15475,8 +15487,8 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59">
-      <c r="A59" s="10" t="s">
-        <v>89</v>
+      <c r="A59" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -15485,8 +15497,8 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60">
-      <c r="A60" s="10" t="s">
-        <v>90</v>
+      <c r="A60" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -15495,8 +15507,8 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="s">
-        <v>91</v>
+      <c r="A61" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -15505,8 +15517,8 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="s">
-        <v>92</v>
+      <c r="A62" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -15515,8 +15527,8 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
-        <v>93</v>
+      <c r="A63" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -15525,8 +15537,8 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
-        <v>94</v>
+      <c r="A64" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -15535,8 +15547,8 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="s">
-        <v>95</v>
+      <c r="A65" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -15545,36 +15557,36 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="s">
-        <v>96</v>
+      <c r="A66" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B66" s="1"/>
-      <c r="C66" s="10" t="s">
-        <v>13</v>
+      <c r="C66" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
-        <v>97</v>
+      <c r="A67" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="1"/>
-      <c r="C67" s="10" t="s">
-        <v>13</v>
+      <c r="C67" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="s">
-        <v>98</v>
+      <c r="A68" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="10" t="s">
-        <v>49</v>
+      <c r="C68" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -15600,37 +15612,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>14</v>
+      <c r="A3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -15639,7 +15651,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -15647,20 +15659,20 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>19</v>
+      <c r="A5" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10" t="s">
-        <v>20</v>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
+      <c r="A6" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -15669,8 +15681,8 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>26</v>
+      <c r="A7" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -15679,8 +15691,8 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>27</v>
+      <c r="A8" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -15689,20 +15701,20 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>29</v>
+      <c r="A9" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="10" t="s">
-        <v>13</v>
+      <c r="F9" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>30</v>
+      <c r="A10" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -15711,8 +15723,8 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>36</v>
+      <c r="A11" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -15721,8 +15733,8 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>37</v>
+      <c r="A12" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -15731,8 +15743,8 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="s">
-        <v>38</v>
+      <c r="A13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -15741,8 +15753,8 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>40</v>
+      <c r="A14" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -15751,8 +15763,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
-        <v>43</v>
+      <c r="A15" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -15761,8 +15773,8 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>44</v>
+      <c r="A16" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -15771,8 +15783,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>45</v>
+      <c r="A17" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -15781,8 +15793,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>46</v>
+      <c r="A18" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -15791,32 +15803,32 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
-        <v>47</v>
+      <c r="A19" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="10" t="s">
-        <v>20</v>
+      <c r="E19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>48</v>
+      <c r="A20" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="10" t="s">
-        <v>49</v>
+      <c r="E20" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>50</v>
+      <c r="A21" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -15825,8 +15837,8 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>51</v>
+      <c r="A22" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -15835,8 +15847,8 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>52</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -15845,8 +15857,8 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>53</v>
+      <c r="A24" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -15855,8 +15867,8 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>54</v>
+      <c r="A25" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -15865,8 +15877,8 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
-        <v>55</v>
+      <c r="A26" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -15875,8 +15887,8 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>57</v>
+      <c r="A27" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -15885,20 +15897,20 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="s">
-        <v>58</v>
+      <c r="A28" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="10" t="s">
-        <v>49</v>
+      <c r="E28" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
-        <v>59</v>
+      <c r="A29" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -15907,68 +15919,68 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>60</v>
+      <c r="A30" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="10" t="s">
-        <v>49</v>
+      <c r="E30" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>61</v>
+      <c r="A31" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="10"/>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>62</v>
+      <c r="A32" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="10" t="s">
-        <v>49</v>
+      <c r="F32" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>63</v>
+      <c r="A33" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="10" t="s">
-        <v>49</v>
+      <c r="F33" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="s">
-        <v>64</v>
+      <c r="A34" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="10" t="s">
-        <v>49</v>
+      <c r="F34" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="s">
-        <v>65</v>
+      <c r="A35" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -15977,8 +15989,8 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="s">
-        <v>66</v>
+      <c r="A36" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -15987,8 +15999,8 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="s">
-        <v>67</v>
+      <c r="A37" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -15997,8 +16009,8 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="s">
-        <v>68</v>
+      <c r="A38" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -16007,8 +16019,8 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
-        <v>69</v>
+      <c r="A39" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -16017,8 +16029,8 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
-        <v>70</v>
+      <c r="A40" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -16027,8 +16039,8 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="s">
-        <v>71</v>
+      <c r="A41" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -16037,8 +16049,8 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42">
-      <c r="A42" s="10" t="s">
-        <v>72</v>
+      <c r="A42" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -16047,8 +16059,8 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43">
-      <c r="A43" s="10" t="s">
-        <v>73</v>
+      <c r="A43" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -16057,8 +16069,8 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44">
-      <c r="A44" s="10" t="s">
-        <v>74</v>
+      <c r="A44" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -16067,8 +16079,8 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45">
-      <c r="A45" s="10" t="s">
-        <v>75</v>
+      <c r="A45" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -16077,8 +16089,8 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46">
-      <c r="A46" s="10" t="s">
-        <v>76</v>
+      <c r="A46" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -16087,8 +16099,8 @@
       <c r="F46" s="1"/>
     </row>
     <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>77</v>
+      <c r="A47" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -16097,8 +16109,8 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48">
-      <c r="A48" s="10" t="s">
-        <v>78</v>
+      <c r="A48" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -16107,8 +16119,8 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49">
-      <c r="A49" s="10" t="s">
-        <v>79</v>
+      <c r="A49" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -16117,8 +16129,8 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50">
-      <c r="A50" s="10" t="s">
-        <v>80</v>
+      <c r="A50" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -16127,8 +16139,8 @@
       <c r="F50" s="1"/>
     </row>
     <row r="51">
-      <c r="A51" s="10" t="s">
-        <v>81</v>
+      <c r="A51" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -16137,8 +16149,8 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52">
-      <c r="A52" s="10" t="s">
-        <v>82</v>
+      <c r="A52" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -16147,8 +16159,8 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53">
-      <c r="A53" s="10" t="s">
-        <v>83</v>
+      <c r="A53" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -16157,8 +16169,8 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54">
-      <c r="A54" s="10" t="s">
-        <v>84</v>
+      <c r="A54" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -16167,8 +16179,8 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="s">
-        <v>85</v>
+      <c r="A55" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -16177,8 +16189,8 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
-        <v>86</v>
+      <c r="A56" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -16187,8 +16199,8 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57">
-      <c r="A57" s="10" t="s">
-        <v>87</v>
+      <c r="A57" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -16197,8 +16209,8 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58">
-      <c r="A58" s="10" t="s">
-        <v>88</v>
+      <c r="A58" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -16207,8 +16219,8 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59">
-      <c r="A59" s="10" t="s">
-        <v>89</v>
+      <c r="A59" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -16217,8 +16229,8 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60">
-      <c r="A60" s="10" t="s">
-        <v>90</v>
+      <c r="A60" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -16227,8 +16239,8 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="s">
-        <v>91</v>
+      <c r="A61" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -16237,8 +16249,8 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="s">
-        <v>92</v>
+      <c r="A62" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -16247,8 +16259,8 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
-        <v>93</v>
+      <c r="A63" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -16257,8 +16269,8 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
-        <v>94</v>
+      <c r="A64" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -16267,8 +16279,8 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="s">
-        <v>95</v>
+      <c r="A65" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -16277,36 +16289,36 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="s">
-        <v>96</v>
+      <c r="A66" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B66" s="1"/>
-      <c r="C66" s="10" t="s">
-        <v>13</v>
+      <c r="C66" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
-        <v>97</v>
+      <c r="A67" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="1"/>
-      <c r="C67" s="10" t="s">
-        <v>13</v>
+      <c r="C67" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="s">
-        <v>98</v>
+      <c r="A68" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="10" t="s">
-        <v>49</v>
+      <c r="C68" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>

</xml_diff>